<commit_message>
fixed excel mali cashew
</commit_message>
<xml_diff>
--- a/data/xls/eco/IKMS Transfert Mali Anacarde.xlsx
+++ b/data/xls/eco/IKMS Transfert Mali Anacarde.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="113">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -300,9 +300,6 @@
     <t xml:space="preserve">Receiver Name</t>
   </si>
   <si>
-    <t xml:space="preserve">value (local currency)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Land owners (land fees)</t>
   </si>
   <si>
@@ -312,7 +309,7 @@
     <t xml:space="preserve">Employees (wages)</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial institutions (interests On loans)</t>
+    <t xml:space="preserve">Financial institutions (interests on loans)</t>
   </si>
   <si>
     <t xml:space="preserve">Government (taxes - subsidies)</t>
@@ -529,37 +526,37 @@
         <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>2</v>
@@ -573,37 +570,37 @@
         <v>966470.4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,37 +611,37 @@
         <v>241920</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,37 +652,37 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>1578034.68208093</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,37 +693,37 @@
         <v>27452.25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,37 +734,37 @@
         <v>538214.4140625</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>10857.7292413088</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -778,37 +775,37 @@
         <v>16000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -843,10 +840,10 @@
         <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -860,10 +857,10 @@
         <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>2833493959.98916</v>
@@ -877,10 +874,10 @@
         <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
@@ -894,10 +891,10 @@
         <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>213760000</v>
@@ -911,10 +908,10 @@
         <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>4435200</v>
@@ -928,10 +925,10 @@
         <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>2822400</v>
@@ -945,10 +942,10 @@
         <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>2833333.359375</v>
@@ -962,10 +959,10 @@
         <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>0</v>
@@ -979,10 +976,10 @@
         <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>0</v>
@@ -996,10 +993,10 @@
         <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1013,10 +1010,10 @@
         <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
@@ -1030,10 +1027,10 @@
         <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>1739884393.06358</v>
@@ -1047,10 +1044,10 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>270165000</v>
@@ -1064,10 +1061,10 @@
         <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>1067744000</v>
@@ -1081,10 +1078,10 @@
         <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>27638553600</v>
@@ -1098,10 +1095,10 @@
         <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>29482790400</v>
@@ -1115,10 +1112,10 @@
         <v>52</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>19730000</v>
@@ -1132,10 +1129,10 @@
         <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0</v>
@@ -1149,10 +1146,10 @@
         <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0</v>
@@ -1166,10 +1163,10 @@
         <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>0</v>
@@ -1183,10 +1180,10 @@
         <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
@@ -1200,10 +1197,10 @@
         <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
@@ -1217,10 +1214,10 @@
         <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0</v>
@@ -1234,10 +1231,10 @@
         <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
@@ -1251,10 +1248,10 @@
         <v>50</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>0</v>
@@ -1268,10 +1265,10 @@
         <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>0</v>
@@ -1285,10 +1282,10 @@
         <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>0</v>
@@ -1302,10 +1299,10 @@
         <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>0</v>
@@ -1319,10 +1316,10 @@
         <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>0</v>
@@ -1336,10 +1333,10 @@
         <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0</v>
@@ -1353,10 +1350,10 @@
         <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>0</v>
@@ -1370,10 +1367,10 @@
         <v>47</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>0</v>
@@ -1387,10 +1384,10 @@
         <v>48</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>0</v>
@@ -1404,10 +1401,10 @@
         <v>49</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0</v>
@@ -1421,10 +1418,10 @@
         <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
@@ -1438,10 +1435,10 @@
         <v>51</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
@@ -1455,10 +1452,10 @@
         <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
@@ -1472,10 +1469,10 @@
         <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>0</v>
@@ -1489,10 +1486,10 @@
         <v>55</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>0</v>
@@ -1506,10 +1503,10 @@
         <v>57</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
@@ -1523,10 +1520,10 @@
         <v>58</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>0</v>
@@ -1540,10 +1537,10 @@
         <v>47</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>21143675982.2074</v>
@@ -1557,10 +1554,10 @@
         <v>48</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>10108875</v>
@@ -1574,10 +1571,10 @@
         <v>49</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>-306144000</v>
@@ -1591,10 +1588,10 @@
         <v>50</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>460051200</v>
@@ -1608,10 +1605,10 @@
         <v>51</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>71164800</v>
@@ -1625,10 +1622,10 @@
         <v>52</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>36666.640625</v>
@@ -1642,10 +1639,10 @@
         <v>53</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E48" s="2" t="n">
         <v>0</v>
@@ -1659,10 +1656,10 @@
         <v>55</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E49" s="2" t="n">
         <v>0</v>
@@ -1676,10 +1673,10 @@
         <v>57</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0</v>
@@ -1693,10 +1690,10 @@
         <v>58</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E51" s="2" t="n">
         <v>0</v>
@@ -1710,10 +1707,10 @@
         <v>47</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E52" s="2" t="n">
         <v>28564800000</v>
@@ -1727,10 +1724,10 @@
         <v>48</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E53" s="2" t="n">
         <v>294000000</v>
@@ -1744,10 +1741,10 @@
         <v>49</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E54" s="2" t="n">
         <v>1344000000</v>
@@ -1761,10 +1758,10 @@
         <v>50</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>28224000000</v>
@@ -1778,10 +1775,10 @@
         <v>51</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E56" s="2" t="n">
         <v>30240000000</v>
@@ -1795,10 +1792,10 @@
         <v>52</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E57" s="2" t="n">
         <v>30600000</v>
@@ -1812,10 +1809,10 @@
         <v>53</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E58" s="2" t="n">
         <v>0</v>
@@ -1829,10 +1826,10 @@
         <v>55</v>
       </c>
       <c r="C59" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E59" s="2" t="n">
         <v>0</v>
@@ -1846,10 +1843,10 @@
         <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E60" s="2" t="n">
         <v>0</v>
@@ -1863,10 +1860,10 @@
         <v>58</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E61" s="2" t="n">
         <v>0</v>
@@ -1880,10 +1877,10 @@
         <v>47</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E62" s="2" t="n">
         <v>0</v>
@@ -1897,10 +1894,10 @@
         <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E63" s="2" t="n">
         <v>0</v>
@@ -1914,10 +1911,10 @@
         <v>49</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E64" s="2" t="n">
         <v>0</v>
@@ -1931,10 +1928,10 @@
         <v>50</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E65" s="2" t="n">
         <v>0</v>
@@ -1948,10 +1945,10 @@
         <v>51</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E66" s="2" t="n">
         <v>0</v>
@@ -1965,10 +1962,10 @@
         <v>52</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E67" s="2" t="n">
         <v>0</v>
@@ -1982,10 +1979,10 @@
         <v>53</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E68" s="2" t="n">
         <v>0</v>
@@ -1999,10 +1996,10 @@
         <v>55</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E69" s="2" t="n">
         <v>0</v>
@@ -2016,10 +2013,10 @@
         <v>57</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E70" s="2" t="n">
         <v>0</v>
@@ -2033,10 +2030,10 @@
         <v>58</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E71" s="2" t="n">
         <v>0</v>
@@ -2050,10 +2047,10 @@
         <v>47</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E72" s="2" t="n">
         <v>0</v>
@@ -2067,10 +2064,10 @@
         <v>48</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E73" s="2" t="n">
         <v>0</v>
@@ -2084,10 +2081,10 @@
         <v>49</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E74" s="2" t="n">
         <v>0</v>
@@ -2101,10 +2098,10 @@
         <v>50</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E75" s="2" t="n">
         <v>0</v>
@@ -2118,10 +2115,10 @@
         <v>51</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E76" s="2" t="n">
         <v>62899200</v>
@@ -2135,10 +2132,10 @@
         <v>52</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E77" s="2" t="n">
         <v>0</v>
@@ -2152,10 +2149,10 @@
         <v>53</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E78" s="2" t="n">
         <v>0</v>
@@ -2169,10 +2166,10 @@
         <v>55</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E79" s="2" t="n">
         <v>0</v>
@@ -2186,10 +2183,10 @@
         <v>57</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E80" s="2" t="n">
         <v>0</v>
@@ -2203,10 +2200,10 @@
         <v>58</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E81" s="2" t="n">
         <v>0</v>
@@ -2220,10 +2217,10 @@
         <v>47</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E82" s="2" t="n">
         <v>2367052023.12139</v>
@@ -2237,10 +2234,10 @@
         <v>48</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E83" s="2" t="n">
         <v>13726125</v>
@@ -2254,10 +2251,10 @@
         <v>49</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E84" s="2" t="n">
         <v>368640000</v>
@@ -2271,10 +2268,10 @@
         <v>50</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E85" s="2" t="n">
         <v>120960000</v>
@@ -2288,10 +2285,10 @@
         <v>51</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E86" s="2" t="n">
         <v>483235200</v>
@@ -2305,10 +2302,10 @@
         <v>52</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E87" s="2" t="n">
         <v>8000000</v>
@@ -2322,10 +2319,10 @@
         <v>53</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E88" s="2" t="n">
         <v>0</v>
@@ -2339,10 +2336,10 @@
         <v>55</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E89" s="2" t="n">
         <v>0</v>
@@ -2356,10 +2353,10 @@
         <v>57</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E90" s="2" t="n">
         <v>0</v>
@@ -2373,10 +2370,10 @@
         <v>58</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E91" s="2" t="n">
         <v>0</v>
@@ -2423,11 +2420,11 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.40234375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="21.41015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3509,11 +3506,14 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.22"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3523,7 +3523,7 @@
         <v>88</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3594,7 +3594,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0</v>
@@ -3602,7 +3602,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>3057344893.34854</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>3361613348.12139</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>62899200</v>

</xml_diff>